<commit_message>
more changes for better formatting
</commit_message>
<xml_diff>
--- a/data/UG/CE-BTech.xlsx
+++ b/data/UG/CE-BTech.xlsx
@@ -1544,7 +1544,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="1" sqref="C:C A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1661,7 +1661,7 @@
   <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="1" sqref="C:C E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3000,7 +3000,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3566,7 +3566,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="C:C A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3662,7 +3662,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="C:C A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3922,7 +3922,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="C:C A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4172,7 +4172,7 @@
   <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D41" activeCellId="0" sqref="D41"/>
+      <selection pane="topLeft" activeCell="D41" activeCellId="1" sqref="C:C D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>